<commit_message>
update scripts with 7 steps and all data
</commit_message>
<xml_diff>
--- a/data/input/trajetoria_montada.xlsx
+++ b/data/input/trajetoria_montada.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelsonthony/Documents/projects/trajectory-analysis/data/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelsonthony/Documents/projects/trajectory-analysis/data/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8703131-B402-B342-898F-84C555BA696D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9575E0-1402-8A42-8440-08A74CE0FEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18260" yWindow="980" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20600" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTrajet" sheetId="1" r:id="rId1"/>
@@ -6496,9 +6496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>